<commit_message>
added files currently working with for timesheet migration
</commit_message>
<xml_diff>
--- a/Hands-on Projects/Timesheet Migration/Timesheets/Karabo Tsaoane/Karabo_Tsaoane_April_FinalWeek.xlsx
+++ b/Hands-on Projects/Timesheet Migration/Timesheets/Karabo Tsaoane/Karabo_Tsaoane_April_FinalWeek.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karabo Tsaoane\Documents\Work\TimeSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scGradsGithub\Hands-on Projects\Timesheet Migration\Timesheets\Karabo Tsaoane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892BD77D-047C-46F2-A6A6-FBB1D8C5C210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4CEEDC-8BA8-40F3-BB02-DFC9D3D25CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C8F8026-B005-4B08-94D3-371A77F74D8F}"/>
   </bookViews>
@@ -23,6 +23,9 @@
     <sheet name="Leave" sheetId="9" r:id="rId8"/>
     <sheet name="Key" sheetId="2" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="TSheet">Apr!$A$8:$J$38</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3488,8 +3491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B63D3D5-6C83-45F2-B2A7-43EE15BF1EF3}">
   <dimension ref="A5:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -10610,15 +10613,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAB60783-D76F-43A9-98C7-BB79EB51704F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAB60783-D76F-43A9-98C7-BB79EB51704F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d277ce56-8de3-43c1-b9ce-ff5033dad840"/>
+    <ds:schemaRef ds:uri="0b8b2123-f09a-47bf-9044-f6e489c8d7a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20201E82-F35A-4134-A060-60C45DDDE0C7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20201E82-F35A-4134-A060-60C45DDDE0C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29C9CCE9-023C-4D8F-A6C9-36AB949B7B72}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29C9CCE9-023C-4D8F-A6C9-36AB949B7B72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d277ce56-8de3-43c1-b9ce-ff5033dad840"/>
+    <ds:schemaRef ds:uri="0b8b2123-f09a-47bf-9044-f6e489c8d7a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
completed timesheet migration without proper checks(need to do)
</commit_message>
<xml_diff>
--- a/Hands-on Projects/Timesheet Migration/Timesheets/Karabo Tsaoane/Karabo_Tsaoane_April_FinalWeek.xlsx
+++ b/Hands-on Projects/Timesheet Migration/Timesheets/Karabo Tsaoane/Karabo_Tsaoane_April_FinalWeek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scGradsGithub\Hands-on Projects\Timesheet Migration\Timesheets\Karabo Tsaoane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4CEEDC-8BA8-40F3-BB02-DFC9D3D25CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A182B-3659-474F-913B-5C9BFBC913D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C8F8026-B005-4B08-94D3-371A77F74D8F}"/>
   </bookViews>
@@ -3492,7 +3492,7 @@
   <dimension ref="A5:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:J38"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>